<commit_message>
excel to xml 3
</commit_message>
<xml_diff>
--- a/OuterConfigData/Excel/自定义配置.xlsx
+++ b/OuterConfigData/Excel/自定义配置.xlsx
@@ -13,30 +13,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>SubID</t>
+  </si>
+  <si>
     <t>名字</t>
   </si>
   <si>
+    <t>list</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
-    <t>2333</t>
+    <t>5050</t>
+  </si>
+  <si>
+    <t>2000333</t>
   </si>
   <si>
     <t>TestCustomList0</t>
   </si>
   <si>
-    <t>10000</t>
+    <t>2000334</t>
+  </si>
+  <si>
+    <t>2000335</t>
+  </si>
+  <si>
+    <t>5051</t>
+  </si>
+  <si>
+    <t>TestCustomList1</t>
+  </si>
+  <si>
+    <t>5052</t>
+  </si>
+  <si>
+    <t>TestCustomList2</t>
+  </si>
+  <si>
+    <t>5053</t>
+  </si>
+  <si>
+    <t>TestCustomList3</t>
+  </si>
+  <si>
+    <t>5054</t>
+  </si>
+  <si>
+    <t>TestCustomList4</t>
   </si>
   <si>
     <t>CustomDataStructure0</t>
+  </si>
+  <si>
+    <t>CustomDataStructure1</t>
+  </si>
+  <si>
+    <t>CustomDataStructure2</t>
+  </si>
+  <si>
+    <t>CustomDataStructure3</t>
+  </si>
+  <si>
+    <t>CustomDataStructure4</t>
   </si>
 </sst>
 </file>
@@ -70,8 +118,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -82,38 +136,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7619955880301" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" style="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1" style="1"/>
+    <col min="3" max="16384" width="14.7619955880301" customWidth="1" style="1"/>
+    <col min="4" max="16384" width="9.140625" customWidth="1" style="1"/>
+    <col min="5" max="16384" width="9.140625" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -123,38 +343,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.2497188023158" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" style="2"/>
+    <col min="2" max="16384" width="20.2497188023158" customWidth="1" style="2"/>
+    <col min="3" max="16384" width="9.140625" customWidth="1" style="2"/>
+    <col min="4" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>